<commit_message>
commit báo cáo đơn giá
</commit_message>
<xml_diff>
--- a/QuanLyThueDat.WebApp/Assets/Template/MauBaoCaoThongBaoTienThueDat.xlsx
+++ b/QuanLyThueDat.WebApp/Assets/Template/MauBaoCaoThongBaoTienThueDat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNPT\QuanLyThueDat\QuanLyThueDat\QuanLyThueDat.WebApp\Assets\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E45A4-551E-4F11-9B63-48EBBC57CA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E0952B-4EA5-4E43-9A57-BEBFE4B86F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>UBND TỈNH NGHỆ AN</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Vị trí thửa đất</t>
+  </si>
+  <si>
+    <t>Ngày thông báo</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,11 +533,11 @@
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -550,9 +553,10 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="2"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -568,9 +572,10 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="2"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -584,9 +589,10 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -603,8 +609,9 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
@@ -634,11 +641,12 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="10"/>
+      <c r="O5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="13"/>
       <c r="C6" s="10"/>
@@ -657,29 +665,32 @@
       <c r="J6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A4:O4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J5:N5"/>
     <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>